<commit_message>
user tracing on RUD operation done, adding name panel on UI done, WIP adding jwt auth on all API
</commit_message>
<xml_diff>
--- a/excel_import/endtest_report_template.xlsx
+++ b/excel_import/endtest_report_template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://johnsonoutdoorsinc-my.sharepoint.com/personal/david_zhang_johnsonoutdoors_com/Documents/Documents/My Files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://johnsonoutdoorsinc-my.sharepoint.com/personal/david_zhang_johnsonoutdoors_com/Documents/David's Stuff/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="281" documentId="13_ncr:1_{A1CECE6E-458F-422C-A05E-4186ECEC6448}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ADA9D05A-64B7-4D88-83F2-A652D8528A2C}"/>
+  <xr:revisionPtr revIDLastSave="296" documentId="13_ncr:1_{A1CECE6E-458F-422C-A05E-4186ECEC6448}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EE58CBC7-269F-48DD-A287-C9FD4D2F5F4D}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Part Number :</t>
   </si>
@@ -56,6 +56,9 @@
   </si>
   <si>
     <t>Data Matrix</t>
+  </si>
+  <si>
+    <t>Created By</t>
   </si>
 </sst>
 </file>
@@ -176,7 +179,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -231,6 +234,12 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="22" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -240,17 +249,8 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="22" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -572,7 +572,7 @@
   <dimension ref="B1:J11"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -580,9 +580,9 @@
     <col min="1" max="1" width="5.140625" style="19" customWidth="1"/>
     <col min="2" max="3" width="22.42578125" style="21" customWidth="1"/>
     <col min="4" max="4" width="19.28515625" style="21" customWidth="1"/>
-    <col min="5" max="5" width="21.140625" style="22" customWidth="1"/>
-    <col min="6" max="6" width="4.85546875" style="22" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="26.28515625" style="23" customWidth="1"/>
+    <col min="5" max="5" width="24" style="22" customWidth="1"/>
+    <col min="6" max="6" width="17.5703125" style="22" customWidth="1"/>
+    <col min="7" max="7" width="22.5703125" style="23" customWidth="1"/>
     <col min="8" max="8" width="22.140625" style="18" customWidth="1"/>
     <col min="9" max="9" width="12.5703125" style="18" customWidth="1"/>
     <col min="10" max="10" width="22.7109375" style="18" customWidth="1"/>
@@ -602,14 +602,14 @@
       <c r="J1" s="5"/>
     </row>
     <row r="2" spans="2:10" s="1" customFormat="1" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="26"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="28"/>
       <c r="H2" s="16"/>
       <c r="I2" s="16"/>
       <c r="J2" s="17"/>
@@ -644,10 +644,10 @@
       </c>
       <c r="C5" s="12"/>
       <c r="D5" s="9"/>
-      <c r="E5" s="13" t="s">
+      <c r="F5" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="G5" s="27"/>
+      <c r="G5" s="11"/>
       <c r="J5" s="11"/>
     </row>
     <row r="6" spans="2:10" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -656,10 +656,10 @@
       </c>
       <c r="C6" s="12"/>
       <c r="D6" s="9"/>
-      <c r="E6" s="13" t="s">
+      <c r="F6" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="G6" s="28"/>
+      <c r="G6" s="29"/>
       <c r="J6" s="5"/>
     </row>
     <row r="7" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -673,20 +673,22 @@
       <c r="J7" s="5"/>
     </row>
     <row r="8" spans="2:10" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="29" t="s">
+      <c r="B8" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="29" t="s">
+      <c r="C8" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="29" t="s">
+      <c r="D8" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="29" t="s">
+      <c r="E8" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="29"/>
-      <c r="G8" s="30" t="s">
+      <c r="F8" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" s="25" t="s">
         <v>3</v>
       </c>
       <c r="H8" s="15"/>

</xml_diff>

<commit_message>
Version 1.3.2 : fixed filter view leaktest and endtest report template
</commit_message>
<xml_diff>
--- a/excel_import/endtest_report_template.xlsx
+++ b/excel_import/endtest_report_template.xlsx
@@ -1,26 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://johnsonoutdoorsinc-my.sharepoint.com/personal/david_zhang_johnsonoutdoors_com/Documents/David's Stuff/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://johnsonoutdoorsinc-my.sharepoint.com/personal/david_zhang_johnsonoutdoors_com/Documents/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="296" documentId="13_ncr:1_{A1CECE6E-458F-422C-A05E-4186ECEC6448}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EE58CBC7-269F-48DD-A287-C9FD4D2F5F4D}"/>
+  <xr:revisionPtr revIDLastSave="300" documentId="13_ncr:1_{A1CECE6E-458F-422C-A05E-4186ECEC6448}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4AD4F3F2-A36E-43ED-A9CD-D6C602BD6E56}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Part Number :</t>
   </si>
@@ -59,6 +72,9 @@
   </si>
   <si>
     <t>Created By</t>
+  </si>
+  <si>
+    <t>Result</t>
   </si>
 </sst>
 </file>
@@ -240,6 +256,9 @@
     <xf numFmtId="22" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -248,9 +267,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -569,10 +585,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:J11"/>
+  <dimension ref="B1:K11"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -581,16 +597,17 @@
     <col min="2" max="3" width="22.42578125" style="21" customWidth="1"/>
     <col min="4" max="4" width="19.28515625" style="21" customWidth="1"/>
     <col min="5" max="5" width="24" style="22" customWidth="1"/>
-    <col min="6" max="6" width="17.5703125" style="22" customWidth="1"/>
-    <col min="7" max="7" width="22.5703125" style="23" customWidth="1"/>
-    <col min="8" max="8" width="22.140625" style="18" customWidth="1"/>
-    <col min="9" max="9" width="12.5703125" style="18" customWidth="1"/>
-    <col min="10" max="10" width="22.7109375" style="18" customWidth="1"/>
-    <col min="11" max="11" width="9.140625" style="19" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="19"/>
+    <col min="6" max="6" width="16.140625" style="22" customWidth="1"/>
+    <col min="7" max="7" width="17.5703125" style="22" customWidth="1"/>
+    <col min="8" max="8" width="22.5703125" style="23" customWidth="1"/>
+    <col min="9" max="9" width="22.140625" style="18" customWidth="1"/>
+    <col min="10" max="10" width="12.5703125" style="18" customWidth="1"/>
+    <col min="11" max="11" width="22.7109375" style="18" customWidth="1"/>
+    <col min="12" max="12" width="9.140625" style="19" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" s="1" customFormat="1" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:11" s="1" customFormat="1" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" s="4"/>
       <c r="C1" s="8"/>
       <c r="D1" s="4"/>
@@ -599,22 +616,24 @@
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
-      <c r="J1" s="5"/>
-    </row>
-    <row r="2" spans="2:10" s="1" customFormat="1" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="26" t="s">
+      <c r="J1" s="2"/>
+      <c r="K1" s="5"/>
+    </row>
+    <row r="2" spans="2:11" s="1" customFormat="1" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
       <c r="G2" s="28"/>
-      <c r="H2" s="16"/>
+      <c r="H2" s="29"/>
       <c r="I2" s="16"/>
-      <c r="J2" s="17"/>
-    </row>
-    <row r="3" spans="2:10" s="7" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J2" s="16"/>
+      <c r="K2" s="17"/>
+    </row>
+    <row r="3" spans="2:11" s="7" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="13" t="s">
         <v>5</v>
       </c>
@@ -623,10 +642,11 @@
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="5"/>
-    </row>
-    <row r="4" spans="2:10" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I3" s="6"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="5"/>
+    </row>
+    <row r="4" spans="2:11" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="13" t="s">
         <v>6</v>
       </c>
@@ -635,34 +655,37 @@
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="5"/>
-    </row>
-    <row r="5" spans="2:10" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H4" s="2"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="5"/>
+    </row>
+    <row r="5" spans="2:11" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="14" t="s">
         <v>0</v>
       </c>
       <c r="C5" s="12"/>
       <c r="D5" s="9"/>
-      <c r="F5" s="13" t="s">
+      <c r="F5" s="8"/>
+      <c r="G5" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="G5" s="11"/>
-      <c r="J5" s="11"/>
-    </row>
-    <row r="6" spans="2:10" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H5" s="11"/>
+      <c r="K5" s="11"/>
+    </row>
+    <row r="6" spans="2:11" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="14" t="s">
         <v>1</v>
       </c>
       <c r="C6" s="12"/>
       <c r="D6" s="9"/>
-      <c r="F6" s="13" t="s">
+      <c r="F6" s="8"/>
+      <c r="G6" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="G6" s="29"/>
-      <c r="J6" s="5"/>
-    </row>
-    <row r="7" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H6" s="26"/>
+      <c r="K6" s="5"/>
+    </row>
+    <row r="7" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
       <c r="D7" s="8"/>
@@ -670,9 +693,10 @@
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
-      <c r="J7" s="5"/>
-    </row>
-    <row r="8" spans="2:10" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I7" s="2"/>
+      <c r="K7" s="5"/>
+    </row>
+    <row r="8" spans="2:11" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="24" t="s">
         <v>2</v>
       </c>
@@ -685,32 +709,35 @@
       <c r="E8" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="25" t="s">
+      <c r="F8" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="G8" s="25" t="s">
+      <c r="H8" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="H8" s="15"/>
-    </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I8" s="15"/>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B9" s="20"/>
       <c r="C9" s="20"/>
       <c r="D9" s="20"/>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B10" s="20"/>
       <c r="C10" s="20"/>
       <c r="D10" s="20"/>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B11" s="20"/>
       <c r="C11" s="20"/>
       <c r="D11" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="B2:H2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="67" orientation="landscape" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>

</xml_diff>